<commit_message>
Resolvedor de cobertura de conjuntos via SAT
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\Downloads\Nova pasta\fs3mod\X3CReducerToSAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49BB0D76-C1DF-4145-9694-A04A577BD27C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFDAE35B-56AC-4B4F-A3B4-02CBD29D1FA8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{93CF00ED-1E8B-48BB-8FD6-89C75F28B121}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Instancias</t>
   </si>
@@ -61,6 +62,15 @@
   </si>
   <si>
     <t>9, 13, 27, 28, 33, 45, 69, 75, 77, 102, 107, 148, 164, 199, 240, 243, 316, 371</t>
+  </si>
+  <si>
+    <t>Numero de Clausulas</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>(+10h)</t>
   </si>
 </sst>
 </file>
@@ -105,7 +115,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -141,14 +154,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7DA91DA-A860-4AE9-94FF-2B69C85DE0AB}" name="Tabela1" displayName="Tabela1" ref="A2:F7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A2:F7" xr:uid="{D5BFD406-10A9-4BA7-97A3-525EE8FB7F47}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{98BF6FA6-C526-457E-9A98-72C0D5F9092D}" name="Instancias" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{5067BFFA-A20F-4CDC-8130-E9008C147270}" name="Numero de elementos X" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{FFC4536E-EA47-4121-BDD4-D85A33892DF1}" name="Numero de subconjuntos" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{B18B0895-3291-49AA-876F-4DEB38BA197B}" name="SAT" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E9A54F30-C990-4AA4-9685-A7BD281D7C82}" name="Tempo de Execução(s)" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7DA91DA-A860-4AE9-94FF-2B69C85DE0AB}" name="Tabela1" displayName="Tabela1" ref="A2:G8" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A2:G8" xr:uid="{D5BFD406-10A9-4BA7-97A3-525EE8FB7F47}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{98BF6FA6-C526-457E-9A98-72C0D5F9092D}" name="Instancias" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{5067BFFA-A20F-4CDC-8130-E9008C147270}" name="Numero de elementos X" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{FFC4536E-EA47-4121-BDD4-D85A33892DF1}" name="Numero de subconjuntos" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{6D9C693A-52E4-4808-90BB-E4F54A6E44B4}" name="Numero de Clausulas" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{B18B0895-3291-49AA-876F-4DEB38BA197B}" name="SAT" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{E9A54F30-C990-4AA4-9685-A7BD281D7C82}" name="Tempo de Execução(s)" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{D36776E8-D6E6-42EB-90CC-FFC8DC6BB51E}" name="Subconjuntos Resposta"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -452,22 +466,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7196EB-AAC7-4602-A245-7F2EB481C979}">
-  <dimension ref="A2:F8"/>
+  <dimension ref="A2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="6" width="32" customWidth="1"/>
+    <col min="3" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,16 +492,19 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -497,17 +514,20 @@
       <c r="C3" s="1">
         <v>254</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="1">
+        <v>10876</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>0.23400000000000001</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -517,14 +537,17 @@
       <c r="C4" s="1">
         <v>209</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="1">
+        <v>2151</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>0.17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -534,17 +557,20 @@
       <c r="C5" s="1">
         <v>454</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="1">
+        <v>8121</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>0.38</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -554,17 +580,20 @@
       <c r="C6" s="1">
         <v>411</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="1">
+        <v>21299</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>0.247</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -574,22 +603,38 @@
       <c r="C7" s="1">
         <v>408</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="1">
+        <v>13796</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>0.19600000000000001</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>387</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1953</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44833</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>